<commit_message>
feito o tratamento e analise
</commit_message>
<xml_diff>
--- a/ScrapingProcessador/processadores_filtrados.xlsx
+++ b/ScrapingProcessador/processadores_filtrados.xlsx
@@ -486,20 +486,14 @@
           <t>Processador AMD Ryzen 7 5700X, 3.4GHz (4.6GHz Max Turbo), Cache 36MB, AM4, Sem Vídeo - 100-100000926WOF</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1.319,99</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2.840,90</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Restam 80 unid.</t>
-        </is>
+      <c r="B2" t="n">
+        <v>1319.99</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2840.9</v>
+      </c>
+      <c r="D2" t="n">
+        <v>80</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -508,7 +502,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Ryzen 7 5700X,</t>
+          <t>Ryzen 7 5700X</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -527,20 +521,14 @@
           <t>Processador AMD Ryzen 5 9600X, 3.9 GHz (5.4 GHz), Cache 32 MB, 6 Núcleos, 12 Threads, AM5 - 100-100001405WOF</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1.649,99</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2.173,90</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Restam 47 unid.</t>
-        </is>
+      <c r="B3" t="n">
+        <v>1649.99</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2173.9</v>
+      </c>
+      <c r="D3" t="n">
+        <v>47</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -549,14 +537,18 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Ryzen 5 9600X,</t>
+          <t>Ryzen 5 9600X</t>
         </is>
       </c>
       <c r="G3" t="n">
         <v>3.9</v>
       </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
+      <c r="H3" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I3" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -564,20 +556,14 @@
           <t>Processador Intel Core i5-14600K, 14ª Geração, 5.3 GHz Max Turbo, Cache 24MB, 14 Núcleos, 20 Threads, LGA1700 - BX8071514600K</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1.749,99</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2.753,40</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Restam 99 unid.</t>
-        </is>
+      <c r="B4" t="n">
+        <v>1749.99</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2753.4</v>
+      </c>
+      <c r="D4" t="n">
+        <v>99</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -586,13 +572,15 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Core i5-14600K,</t>
+          <t>Core i5-14600K</t>
         </is>
       </c>
       <c r="G4" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H4" t="n">
         <v>5.3</v>
       </c>
-      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
         <v>24</v>
       </c>
@@ -603,20 +591,14 @@
           <t>Processador Intel Core i7-12700F, 2.1GHz (4.9GHz Max Turbo), Cache 25MB, LGA 1700 - BX8071512700F</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1.699,99</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2.282,59</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Restam 98 unid.</t>
-        </is>
+      <c r="B5" t="n">
+        <v>1699.99</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2282.59</v>
+      </c>
+      <c r="D5" t="n">
+        <v>98</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -625,7 +607,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Core i7-12700F,</t>
+          <t>Core i7-12700F</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -644,20 +626,14 @@
           <t>Processador AMD Ryzen 7 8700G, 4.2GHz (5.1GHz Max Turbo), Cache 8MB, Octa-Core, 16 Threads, AM5, Vídeo Integrado - 100-100001236BOX</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>1.949,99</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2.282,60</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Restam 84 unid.</t>
-        </is>
+      <c r="B6" t="n">
+        <v>1949.99</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2282.6</v>
+      </c>
+      <c r="D6" t="n">
+        <v>84</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -666,7 +642,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Ryzen 7 8700G,</t>
+          <t>Ryzen 7 8700G</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -685,20 +661,14 @@
           <t>Processador AMD Ryzen 9 9900X, 4.4 GHz (5.6 GHz), Cache 64 MB, 12 Núcleos, 24 Threads, AM5 - 100-100000662WOF</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2.899,99</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>4.705,87</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Restam 97 unid.</t>
-        </is>
+      <c r="B7" t="n">
+        <v>2899.99</v>
+      </c>
+      <c r="C7" t="n">
+        <v>4705.87</v>
+      </c>
+      <c r="D7" t="n">
+        <v>97</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -707,14 +677,18 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Ryzen 9 9900X,</t>
+          <t>Ryzen 9 9900X</t>
         </is>
       </c>
       <c r="G7" t="n">
         <v>4.4</v>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
+      <c r="H7" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I7" t="n">
+        <v>64</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -722,20 +696,14 @@
           <t>Processador AMD Ryzen 7 5700, 3.7 GHz (4.6GHz Max Turbo), Cache 4MB, 8 Núcleos, 16 Threads, AM4 - 100-100000743BOX</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>1.099,99</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1.444,43</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Restam 41 unid.</t>
-        </is>
+      <c r="B8" t="n">
+        <v>1099.99</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1444.43</v>
+      </c>
+      <c r="D8" t="n">
+        <v>41</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -744,7 +712,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Ryzen 7 5700,</t>
+          <t>Ryzen 7 5700</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -763,20 +731,14 @@
           <t>Processador AMD Ryzen 9 9950x3d, 4,4 GHz, (Máx Boos Clock Até 5,5 GHz), Cache 144MB, 16 Núcleos, Threads 32, AM5 - 100-100000719WOF</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>5.299,99</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>7.777,77</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Restam 33 unid.</t>
-        </is>
+      <c r="B9" t="n">
+        <v>5299.99</v>
+      </c>
+      <c r="C9" t="n">
+        <v>7777.77</v>
+      </c>
+      <c r="D9" t="n">
+        <v>33</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -785,13 +747,15 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Ryzen 9 9950x3d,</t>
+          <t>Ryzen 9 9950x3d</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>4</v>
-      </c>
-      <c r="H9" t="inlineStr"/>
+        <v>4.4</v>
+      </c>
+      <c r="H9" t="n">
+        <v>5.05</v>
+      </c>
       <c r="I9" t="n">
         <v>144</v>
       </c>
@@ -802,20 +766,14 @@
           <t>Processador Intel Core i5-10400, 2.9GHz (4.3GHz Max Turbo), Cache 12MB, LGA 1200 - BX8070110400</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>949,99</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1.177,76</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Restam 94 unid.</t>
-        </is>
+      <c r="B10" t="n">
+        <v>949.99</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1177.76</v>
+      </c>
+      <c r="D10" t="n">
+        <v>94</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -824,7 +782,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Core i5-10400,</t>
+          <t>Core i5-10400</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -843,20 +801,14 @@
           <t>Processador Intel Core i5-12600KF, 3.7GHz (4.9Ghz Max Turbo), Cache 20MB, Quad Core, 16 Threads, LGA 1700 - BX8071512600KF</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1.199,99</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1.555,55</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Restam 81 unid.</t>
-        </is>
+      <c r="B11" t="n">
+        <v>1199.99</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1555.55</v>
+      </c>
+      <c r="D11" t="n">
+        <v>81</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -865,13 +817,15 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Core i5-12600KF,</t>
+          <t>Core i5-12600KF</t>
         </is>
       </c>
       <c r="G11" t="n">
         <v>3.7</v>
       </c>
-      <c r="H11" t="inlineStr"/>
+      <c r="H11" t="n">
+        <v>4.9</v>
+      </c>
       <c r="I11" t="n">
         <v>20</v>
       </c>
@@ -882,20 +836,14 @@
           <t>Processador Intel Core i5-13400F, 4.6GHz Max Turbo, Cache 20MB, 10 Núcleos, 16 Threads, LGA 1700 - BX8071513400F</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1.199,99</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1.847,81</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Restam 33 unid.</t>
-        </is>
+      <c r="B12" t="n">
+        <v>1199.99</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1847.81</v>
+      </c>
+      <c r="D12" t="n">
+        <v>33</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -904,13 +852,15 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Core i5-13400F,</t>
+          <t>Core i5-13400F</t>
         </is>
       </c>
       <c r="G12" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H12" t="n">
         <v>4.6</v>
       </c>
-      <c r="H12" t="inlineStr"/>
       <c r="I12" t="n">
         <v>20</v>
       </c>
@@ -921,20 +871,14 @@
           <t>Processador AMD Ryzen 7 5800X, 3.8GHz (4.7GHz Max Turbo), Cache 36MB, Octa Core, 16 Threads, AM4 - 100-100000063WOF</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>1.669,99</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>3.695,63</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Restam 90 unid.</t>
-        </is>
+      <c r="B13" t="n">
+        <v>1669.99</v>
+      </c>
+      <c r="C13" t="n">
+        <v>3695.63</v>
+      </c>
+      <c r="D13" t="n">
+        <v>90</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -943,7 +887,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Ryzen 7 5800X,</t>
+          <t>Ryzen 7 5800X</t>
         </is>
       </c>
       <c r="G13" t="n">
@@ -962,20 +906,14 @@
           <t>Processador Intel Core I3-10100, 3.60GHz (4.3GHz Turbo), Cache 6MB, LGA 1200 - BX8070110100</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>679,00</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>810,90</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Restam 67 unid.</t>
-        </is>
+      <c r="B14" t="n">
+        <v>679</v>
+      </c>
+      <c r="C14" t="n">
+        <v>810.9</v>
+      </c>
+      <c r="D14" t="n">
+        <v>67</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -984,14 +922,14 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Core I3-1</t>
+          <t>Core I3-10100</t>
         </is>
       </c>
       <c r="G14" t="n">
         <v>3.6</v>
       </c>
       <c r="H14" t="n">
-        <v>4.3</v>
+        <v>5.05</v>
       </c>
       <c r="I14" t="n">
         <v>6</v>
@@ -1003,20 +941,14 @@
           <t>Processador Intel Core i5-14600KF, 14ª Geração, 5.3 GHz Max Turbo, Cache 24MB, 14 Núcleos, 20 Threads, LGA1700 - BX8071514600KF</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>1.599,99</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>2.065,21</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Restam 19 unid.</t>
-        </is>
+      <c r="B15" t="n">
+        <v>1599.99</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2065.21</v>
+      </c>
+      <c r="D15" t="n">
+        <v>19</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -1025,13 +957,15 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Core i5-14600KF,</t>
+          <t>Core i5-14600KF</t>
         </is>
       </c>
       <c r="G15" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H15" t="n">
         <v>5.3</v>
       </c>
-      <c r="H15" t="inlineStr"/>
       <c r="I15" t="n">
         <v>24</v>
       </c>
@@ -1042,20 +976,14 @@
           <t>Processador Intel Core I5 - 12400F, 2.5GHz (4.4GHz Turbo), Cache 7,5MB, 12 Threads, Hexa Core, LGA 1700 - BX8071512400F</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>769,00</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>1.055,90</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Restam 26 unid.</t>
-        </is>
+      <c r="B16" t="n">
+        <v>769</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1055.9</v>
+      </c>
+      <c r="D16" t="n">
+        <v>26</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1064,16 +992,18 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Core I5 - 12400F,</t>
+          <t>Core I5</t>
         </is>
       </c>
       <c r="G16" t="n">
         <v>2.5</v>
       </c>
       <c r="H16" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="I16" t="inlineStr"/>
+        <v>5.05</v>
+      </c>
+      <c r="I16" t="n">
+        <v>27.5</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1081,20 +1011,14 @@
           <t>Processador AMD Ryzen 9 5900XT, 3,3 GHz (4.8 GHz), Cache 64MB, 16 Núcleos, 32 Threads, AM4 - 100-100001581WOF</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>2.259,99</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>2.666,66</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Restam 22 unid.</t>
-        </is>
+      <c r="B17" t="n">
+        <v>2259.99</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2666.66</v>
+      </c>
+      <c r="D17" t="n">
+        <v>22</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1103,13 +1027,15 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Ryzen 9 5900XT,</t>
+          <t>Ryzen 9 5900XT</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>3</v>
-      </c>
-      <c r="H17" t="inlineStr"/>
+        <v>3.3</v>
+      </c>
+      <c r="H17" t="n">
+        <v>5.05</v>
+      </c>
       <c r="I17" t="n">
         <v>64</v>
       </c>
@@ -1120,20 +1046,14 @@
           <t>Processador AMD Ryzen 5 8400F, 4.2 GHz (4.7 GHz Max Turbo), Cache 22MB, AM5, 6 Núcleos, 12 Threads - 100-100001591BOX</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>1.049,99</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>1.444,43</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Restam 45 unid.</t>
-        </is>
+      <c r="B18" t="n">
+        <v>1049.99</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1444.43</v>
+      </c>
+      <c r="D18" t="n">
+        <v>45</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1142,13 +1062,15 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Ryzen 5 8400F,</t>
+          <t>Ryzen 5 8400F</t>
         </is>
       </c>
       <c r="G18" t="n">
         <v>4.2</v>
       </c>
-      <c r="H18" t="inlineStr"/>
+      <c r="H18" t="n">
+        <v>4.7</v>
+      </c>
       <c r="I18" t="n">
         <v>22</v>
       </c>
@@ -1159,20 +1081,14 @@
           <t>Processador Intel Core i3-13100, 4.5GHz Max Turbo, Cache 12MB, 4 Núcleos, 8 Threads, LGA 1700, Vídeo Integrado - BX8071513100</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>849,99</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>1.086,95</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Restam 32 unid.</t>
-        </is>
+      <c r="B19" t="n">
+        <v>849.99</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1086.95</v>
+      </c>
+      <c r="D19" t="n">
+        <v>32</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1181,13 +1097,15 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Core i3-13100,</t>
+          <t>Core i3-13100</t>
         </is>
       </c>
       <c r="G19" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H19" t="n">
         <v>4.5</v>
       </c>
-      <c r="H19" t="inlineStr"/>
       <c r="I19" t="n">
         <v>12</v>
       </c>
@@ -1198,20 +1116,14 @@
           <t>Processador AMD Ryzen 9 9950X, 4.3 GHz (5.7 GHz), Cache 64 MB, 16 Núcleos, 32 Threads, AM5 - 100-100001277WOF</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>3.999,99</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>4.823,52</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Restam 20 unid.</t>
-        </is>
+      <c r="B20" t="n">
+        <v>3999.99</v>
+      </c>
+      <c r="C20" t="n">
+        <v>4823.52</v>
+      </c>
+      <c r="D20" t="n">
+        <v>20</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1220,14 +1132,18 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Ryzen 9 9950X,</t>
+          <t>Ryzen 9 9950X</t>
         </is>
       </c>
       <c r="G20" t="n">
         <v>4.3</v>
       </c>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
+      <c r="H20" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I20" t="n">
+        <v>64</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1235,20 +1151,14 @@
           <t>Processador Intel Core i3-12100, Cache 12MB, 3.3GHz (4.3GHz Max Turbo), LGA 1700, Vídeo Integrado, com Cooler - BX8071512100</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>849,99</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>1.058,81</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Restam 58 unid.</t>
-        </is>
+      <c r="B21" t="n">
+        <v>849.99</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1058.81</v>
+      </c>
+      <c r="D21" t="n">
+        <v>58</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1257,7 +1167,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Core i3-12100,</t>
+          <t>Core i3-12100</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -1276,20 +1186,14 @@
           <t>Processador Intel Core i5-13400, 4.6GHz Max Turbo, Cache 20MB, 10 Núcleos, 16 Threads, LGA 1700, Vídeo Integrado - BX8071513400</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>1.399,99</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>1.704,53</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Restam 77 unid.</t>
-        </is>
+      <c r="B22" t="n">
+        <v>1399.99</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1704.53</v>
+      </c>
+      <c r="D22" t="n">
+        <v>77</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1298,13 +1202,15 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Core i5-13400,</t>
+          <t>Core i5-13400</t>
         </is>
       </c>
       <c r="G22" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H22" t="n">
         <v>4.6</v>
       </c>
-      <c r="H22" t="inlineStr"/>
       <c r="I22" t="n">
         <v>20</v>
       </c>
@@ -1315,20 +1221,14 @@
           <t>Processador Intel Core i9-12900KF, 3.2GHz (5.2GHz Max Turbo), Cache 30MB, 16 Núcleos, 24 Threads, LGA 1700 - BX8071512900KF</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>2.299,99</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>3.333,31</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Restam 29 unid.</t>
-        </is>
+      <c r="B23" t="n">
+        <v>2299.99</v>
+      </c>
+      <c r="C23" t="n">
+        <v>3333.31</v>
+      </c>
+      <c r="D23" t="n">
+        <v>29</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1337,7 +1237,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Core i9-12900KF,</t>
+          <t>Core i9-12900KF</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -1356,20 +1256,14 @@
           <t>Processador AMD Ryzen 9 7900X, 5.6GHz Max Turbo, Cache 76MB, AM5, 12 Núcleos, Vídeo Integrado - 100-100000589WOF</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>2.769,99</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>4.675,23</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Restam 69 unid.</t>
-        </is>
+      <c r="B24" t="n">
+        <v>2769.99</v>
+      </c>
+      <c r="C24" t="n">
+        <v>4675.23</v>
+      </c>
+      <c r="D24" t="n">
+        <v>69</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1378,13 +1272,15 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Ryzen 9 7900X,</t>
+          <t>Ryzen 9 7900X</t>
         </is>
       </c>
       <c r="G24" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H24" t="n">
         <v>5.6</v>
       </c>
-      <c r="H24" t="inlineStr"/>
       <c r="I24" t="n">
         <v>76</v>
       </c>
@@ -1395,20 +1291,14 @@
           <t>Processador Intel Pentium Gold G6400 Processor, 4.00 GHz, Cache 4MB, Dual Core, 4 Threads, LGA1200 - BX80701G6400</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>519,99</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>599,99</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Restam 30 unid.</t>
-        </is>
+      <c r="B25" t="n">
+        <v>519.99</v>
+      </c>
+      <c r="C25" t="n">
+        <v>599.99</v>
+      </c>
+      <c r="D25" t="n">
+        <v>30</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1423,7 +1313,9 @@
       <c r="G25" t="n">
         <v>4</v>
       </c>
-      <c r="H25" t="inlineStr"/>
+      <c r="H25" t="n">
+        <v>5.05</v>
+      </c>
       <c r="I25" t="n">
         <v>4</v>
       </c>
@@ -1434,20 +1326,14 @@
           <t>Processador AMD Ryzen 9 7900, 5.4GHz Max Turbo, Cache 76MB, AM5, 12 Núcleos, Vídeo Integrado - 100-100000590BOX</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>2.649,99</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>3.444,44</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Restam 47 unid.</t>
-        </is>
+      <c r="B26" t="n">
+        <v>2649.99</v>
+      </c>
+      <c r="C26" t="n">
+        <v>3444.44</v>
+      </c>
+      <c r="D26" t="n">
+        <v>47</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1456,13 +1342,15 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Ryzen 9 7900,</t>
+          <t>Ryzen 9 7900</t>
         </is>
       </c>
       <c r="G26" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H26" t="n">
         <v>5.4</v>
       </c>
-      <c r="H26" t="inlineStr"/>
       <c r="I26" t="n">
         <v>76</v>
       </c>
@@ -1473,20 +1361,14 @@
           <t>Processador Intel Core i5-12600K, 3.7GHz (4.9GHz Max Turbo), Cache 20MB, 10 Núcleos, 16 Threads, LGA 1700, Vídeo Integrado - BX8071512600K</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>1.299,99</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>1.835,28</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Restam 79 unid.</t>
-        </is>
+      <c r="B27" t="n">
+        <v>1299.99</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1835.28</v>
+      </c>
+      <c r="D27" t="n">
+        <v>79</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1495,7 +1377,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Core i5-12600K,</t>
+          <t>Core i5-12600K</t>
         </is>
       </c>
       <c r="G27" t="n">
@@ -1514,20 +1396,14 @@
           <t>Processador AMD Ryzen 9 7950X, 5.7GHz Max Turbo, Cache 80MB, AM5, 16 Núcleos, Vídeo Integrado - 100-100000514WOF</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>3.699,99</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>6.930,15</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Restam 85 unid.</t>
-        </is>
+      <c r="B28" t="n">
+        <v>3699.99</v>
+      </c>
+      <c r="C28" t="n">
+        <v>6930.15</v>
+      </c>
+      <c r="D28" t="n">
+        <v>85</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1536,13 +1412,15 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Ryzen 9 7950X,</t>
+          <t>Ryzen 9 7950X</t>
         </is>
       </c>
       <c r="G28" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H28" t="n">
         <v>5.7</v>
       </c>
-      <c r="H28" t="inlineStr"/>
       <c r="I28" t="n">
         <v>80</v>
       </c>
@@ -1553,20 +1431,14 @@
           <t>Processador Intel Core i7-13700F, 5.2GHz Max Turbo, Cache 30MB, 16 Núcleos, 24 Threads, LGA 1700 - BX8071513700F</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>2.299,99</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>3.058,81</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Restam 10 unid.</t>
-        </is>
+      <c r="B29" t="n">
+        <v>2299.99</v>
+      </c>
+      <c r="C29" t="n">
+        <v>3058.81</v>
+      </c>
+      <c r="D29" t="n">
+        <v>10</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1575,13 +1447,15 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Core i7-13700F,</t>
+          <t>Core i7-13700F</t>
         </is>
       </c>
       <c r="G29" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H29" t="n">
         <v>5.2</v>
       </c>
-      <c r="H29" t="inlineStr"/>
       <c r="I29" t="n">
         <v>30</v>
       </c>
@@ -1592,20 +1466,14 @@
           <t>Processador AMD Ryzen 9 9900x3d, 4,4 GHz, (Máx Boos Clock Até 5,5 GHz), Cache 140MB, 12 Núcleos, Threads 24, AM5 - 100-100001368WOF</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>4.199,99</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>7.222,21</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Restam 29 unid.</t>
-        </is>
+      <c r="B30" t="n">
+        <v>4199.99</v>
+      </c>
+      <c r="C30" t="n">
+        <v>7222.21</v>
+      </c>
+      <c r="D30" t="n">
+        <v>29</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1614,13 +1482,15 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Ryzen 9 9900x3d,</t>
+          <t>Ryzen 9 9900x3d</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>4</v>
-      </c>
-      <c r="H30" t="inlineStr"/>
+        <v>4.4</v>
+      </c>
+      <c r="H30" t="n">
+        <v>5.05</v>
+      </c>
       <c r="I30" t="n">
         <v>140</v>
       </c>
@@ -1631,20 +1501,14 @@
           <t>Processador Intel Core i3-10100F, 3.6GHz (4.3GHz Max Boost), Cache 6MB, Quad Core, 8 Threads, LGA 1200 - BX8070110100F</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>499,99</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>624,99</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Restam 13 unid.</t>
-        </is>
+      <c r="B31" t="n">
+        <v>499.99</v>
+      </c>
+      <c r="C31" t="n">
+        <v>624.99</v>
+      </c>
+      <c r="D31" t="n">
+        <v>13</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1653,14 +1517,14 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Core i3-10100F,</t>
+          <t>Core i3-10100F</t>
         </is>
       </c>
       <c r="G31" t="n">
         <v>3.6</v>
       </c>
       <c r="H31" t="n">
-        <v>4.3</v>
+        <v>5.05</v>
       </c>
       <c r="I31" t="n">
         <v>6</v>
@@ -1672,20 +1536,14 @@
           <t>Processador Intel Core i9-13900F, 5.6GHz Max Turbo, Cache 36MB, 24 Núcleos, 32 Threads, LGA 1700 - BX8071513900F</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>2.949,99</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>3.467,39</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>Restam 15 unid.</t>
-        </is>
+      <c r="B32" t="n">
+        <v>2949.99</v>
+      </c>
+      <c r="C32" t="n">
+        <v>3467.39</v>
+      </c>
+      <c r="D32" t="n">
+        <v>15</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1694,13 +1552,15 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Core i9-13900F,</t>
+          <t>Core i9-13900F</t>
         </is>
       </c>
       <c r="G32" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H32" t="n">
         <v>5.6</v>
       </c>
-      <c r="H32" t="inlineStr"/>
       <c r="I32" t="n">
         <v>36</v>
       </c>
@@ -1711,24 +1571,18 @@
           <t>Processador Amd Ryzen 9 9950x3d Am5 4,3ghz 5,7ghz Turbo 16 Cores 32 Threads 144mb S/cooler C/vídeo</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>5.129,90</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>6.443,90</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Restam 9 unid.</t>
-        </is>
+      <c r="B33" t="n">
+        <v>5129.9</v>
+      </c>
+      <c r="C33" t="n">
+        <v>6443.9</v>
+      </c>
+      <c r="D33" t="n">
+        <v>9</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Amd</t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1736,9 +1590,15 @@
           <t>Ryzen 9 9950x3d</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr"/>
+      <c r="G33" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="H33" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I33" t="n">
+        <v>27.5</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1746,20 +1606,14 @@
           <t>Processador Intel Celeron G5905, 3.50 GHz, Cache 4MB, 2 Núcleos, 2 Threads, LGA 1200, Vídeo Integrado - BX80701G5905</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>329,99</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>411,75</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Restam 10 unid.</t>
-        </is>
+      <c r="B34" t="n">
+        <v>329.99</v>
+      </c>
+      <c r="C34" t="n">
+        <v>411.75</v>
+      </c>
+      <c r="D34" t="n">
+        <v>10</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1768,13 +1622,15 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Desconhecido</t>
+          <t>Celeron G5905</t>
         </is>
       </c>
       <c r="G34" t="n">
         <v>3.5</v>
       </c>
-      <c r="H34" t="inlineStr"/>
+      <c r="H34" t="n">
+        <v>5.05</v>
+      </c>
       <c r="I34" t="n">
         <v>4</v>
       </c>
@@ -1785,20 +1641,14 @@
           <t>Processador Intel Pentium Gold G6405, 4.10 GHz, Cache 4MB, Dual Core, 4 Threads, LGA1200 - BX80701G6405</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>529,99</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>636,35</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Restam 10 unid.</t>
-        </is>
+      <c r="B35" t="n">
+        <v>529.99</v>
+      </c>
+      <c r="C35" t="n">
+        <v>636.35</v>
+      </c>
+      <c r="D35" t="n">
+        <v>10</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1813,7 +1663,9 @@
       <c r="G35" t="n">
         <v>4.1</v>
       </c>
-      <c r="H35" t="inlineStr"/>
+      <c r="H35" t="n">
+        <v>5.05</v>
+      </c>
       <c r="I35" t="n">
         <v>4</v>
       </c>
@@ -1824,20 +1676,14 @@
           <t>Processador AMD Ryzen 9 7950X3D, 5.7GHz Max Turbo, Cache 128MB, AM5, 16 Núcleos, Vídeo Integrado - 100-100000908WOF</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>4.999,99</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>6.111,10</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Restam 15 unid.</t>
-        </is>
+      <c r="B36" t="n">
+        <v>4999.99</v>
+      </c>
+      <c r="C36" t="n">
+        <v>6111.1</v>
+      </c>
+      <c r="D36" t="n">
+        <v>15</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1846,13 +1692,15 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Ryzen 9 7950X3D,</t>
+          <t>Ryzen 9 7950X3D</t>
         </is>
       </c>
       <c r="G36" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H36" t="n">
         <v>5.7</v>
       </c>
-      <c r="H36" t="inlineStr"/>
       <c r="I36" t="n">
         <v>128</v>
       </c>
@@ -1863,20 +1711,14 @@
           <t>Processador Intel Core i3-10105F, 3.7GHz (4.4GHz Max Turbo), Cache 6MB, Quad Core, 8 Thread, LGA 1200 - BX8070110105F</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>499,99</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>586,95</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Restam 49 unid.</t>
-        </is>
+      <c r="B37" t="n">
+        <v>499.99</v>
+      </c>
+      <c r="C37" t="n">
+        <v>586.95</v>
+      </c>
+      <c r="D37" t="n">
+        <v>49</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1885,7 +1727,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Core i3-10105F,</t>
+          <t>Core i3-10105F</t>
         </is>
       </c>
       <c r="G37" t="n">
@@ -1904,20 +1746,14 @@
           <t>Processador AMD Ryzen 5 7600X, 5.3GHz, Cache 38MB, AM5, Radeon Graphics - 100-100000593WOF</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>1.644,23</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>2.012,53</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Restam 39 unid.</t>
-        </is>
+      <c r="B38" t="n">
+        <v>1644.23</v>
+      </c>
+      <c r="C38" t="n">
+        <v>2012.53</v>
+      </c>
+      <c r="D38" t="n">
+        <v>39</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1926,13 +1762,15 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Ryzen 5 7600X,</t>
+          <t>Ryzen 5 7600X</t>
         </is>
       </c>
       <c r="G38" t="n">
         <v>5.3</v>
       </c>
-      <c r="H38" t="inlineStr"/>
+      <c r="H38" t="n">
+        <v>5.05</v>
+      </c>
       <c r="I38" t="n">
         <v>38</v>
       </c>
@@ -1943,20 +1781,14 @@
           <t>Processador Intel Core Ultra 7-265K, 5.5GHz, Até 20 Núcleos, Com suporte a PCIe 5.0 e 4.0 e suporte a DDR5 - BX80768265K</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>2.899,99</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>3.977,26</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>Restam 20 unid.</t>
-        </is>
+      <c r="B39" t="n">
+        <v>2899.99</v>
+      </c>
+      <c r="C39" t="n">
+        <v>3977.26</v>
+      </c>
+      <c r="D39" t="n">
+        <v>20</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1965,14 +1797,18 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Ultra 7-265K,</t>
+          <t>Ultra 7</t>
         </is>
       </c>
       <c r="G39" t="n">
         <v>5.5</v>
       </c>
-      <c r="H39" t="inlineStr"/>
-      <c r="I39" t="inlineStr"/>
+      <c r="H39" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I39" t="n">
+        <v>27.5</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1980,20 +1816,14 @@
           <t>Processador Intel Core i9-12900K, 3.2GHz (5.2GHz Max Turbo), Cache 30MB, 16 Núcleos, 24 Threads, LGA 1700, Vídeo Integrado - BX8071512900K</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>2.499,99</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>3.260,86</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>Restam 19 unid.</t>
-        </is>
+      <c r="B40" t="n">
+        <v>2499.99</v>
+      </c>
+      <c r="C40" t="n">
+        <v>3260.86</v>
+      </c>
+      <c r="D40" t="n">
+        <v>19</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -2002,7 +1832,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Core i9-12900K,</t>
+          <t>Core i9-12900K</t>
         </is>
       </c>
       <c r="G40" t="n">
@@ -2021,20 +1851,14 @@
           <t>Processador Intel Core I5-10400F, 2.9GHz (4.3GHz Turbo), Hexa Core, Cache 12MB, LGA 1200 - BX8070110400F</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>749,00</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>913,90</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>Restam 37 unid.</t>
-        </is>
+      <c r="B41" t="n">
+        <v>749</v>
+      </c>
+      <c r="C41" t="n">
+        <v>913.9</v>
+      </c>
+      <c r="D41" t="n">
+        <v>37</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -2043,14 +1867,14 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Core I5-1</t>
+          <t>Core I5-10400F</t>
         </is>
       </c>
       <c r="G41" t="n">
         <v>2.9</v>
       </c>
       <c r="H41" t="n">
-        <v>4.3</v>
+        <v>5.05</v>
       </c>
       <c r="I41" t="n">
         <v>12</v>
@@ -2062,20 +1886,14 @@
           <t>Processador AMD Ryzen Radeon 9 7950X, 2200MHz, Cache 80MB, 1Hexa Core, AM5, Vídeo Integrado - 100-100000514WOF</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>4.054,81</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>4.963,05</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Restam 35 unid.</t>
-        </is>
+      <c r="B42" t="n">
+        <v>4054.81</v>
+      </c>
+      <c r="C42" t="n">
+        <v>4963.05</v>
+      </c>
+      <c r="D42" t="n">
+        <v>35</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2087,8 +1905,12 @@
           <t>Desconhecido</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
+      <c r="G42" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H42" t="n">
+        <v>5.05</v>
+      </c>
       <c r="I42" t="n">
         <v>80</v>
       </c>
@@ -2099,20 +1921,14 @@
           <t>Processador Intel Core I5-12600KF 12ª Geração, 3.7GHz, Cache 20MB, 10 Núcleos, 16 Threads, LGA 1700 - BX8071512600KF</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>1.299,00</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>1.609,90</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Restam 64 unid.</t>
-        </is>
+      <c r="B43" t="n">
+        <v>1299</v>
+      </c>
+      <c r="C43" t="n">
+        <v>1609.9</v>
+      </c>
+      <c r="D43" t="n">
+        <v>64</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -2121,13 +1937,15 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Core I5-1</t>
+          <t>Core I5-12600KF</t>
         </is>
       </c>
       <c r="G43" t="n">
         <v>3.7</v>
       </c>
-      <c r="H43" t="inlineStr"/>
+      <c r="H43" t="n">
+        <v>5.05</v>
+      </c>
       <c r="I43" t="n">
         <v>20</v>
       </c>
@@ -2138,20 +1956,14 @@
           <t>Processador Intel I3-12100F, 3.3GHz, Cache 12MB, Quad Core, 8 Threads, LGA 1700 - BX8071512100F</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>579,00</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>720,90</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Restam 43 unid.</t>
-        </is>
+      <c r="B44" t="n">
+        <v>579</v>
+      </c>
+      <c r="C44" t="n">
+        <v>720.9</v>
+      </c>
+      <c r="D44" t="n">
+        <v>43</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2166,7 +1978,9 @@
       <c r="G44" t="n">
         <v>3.3</v>
       </c>
-      <c r="H44" t="inlineStr"/>
+      <c r="H44" t="n">
+        <v>5.05</v>
+      </c>
       <c r="I44" t="n">
         <v>12</v>
       </c>
@@ -2177,20 +1991,14 @@
           <t>Processador AMD Ryzen 9 7950X3D, 4.2GHz, 5.7GHz, Cache 16MB, AM5, 16 Núcleos, 32threads, Placa de Vídeo, S/ Cooler - 100-100000908WOF</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>5.005,11</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>6.126,21</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>Restam 82 unid.</t>
-        </is>
+      <c r="B45" t="n">
+        <v>5005.11</v>
+      </c>
+      <c r="C45" t="n">
+        <v>6126.21</v>
+      </c>
+      <c r="D45" t="n">
+        <v>82</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -2199,13 +2007,15 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Ryzen 9 7950X3D,</t>
+          <t>Ryzen 9 7950X3D</t>
         </is>
       </c>
       <c r="G45" t="n">
         <v>4.2</v>
       </c>
-      <c r="H45" t="inlineStr"/>
+      <c r="H45" t="n">
+        <v>5.05</v>
+      </c>
       <c r="I45" t="n">
         <v>16</v>
       </c>
@@ -2216,20 +2026,14 @@
           <t>Processador Intel Core I3 14100f, 14ª Geração, 3.5 Ghz, 4.7 Ghz Turbo, Cache 12mb Lga 1700, Sem Vídeo - Bx8071514100f</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>639,00</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>759,90</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Restam 34 unid.</t>
-        </is>
+      <c r="B46" t="n">
+        <v>639</v>
+      </c>
+      <c r="C46" t="n">
+        <v>759.9</v>
+      </c>
+      <c r="D46" t="n">
+        <v>34</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2238,12 +2042,18 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Core I3 14100f,</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr"/>
+          <t>Core I3 14100f</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="H46" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I46" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2251,20 +2061,14 @@
           <t>Processador Intel Core Ultra 7-265KF, 5.5GHz, Até 20 Núcleos, Com suporte a PCIe 5.0 e 4.0 e suporte a DDR5 - BX80768265KF</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>2.899,99</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>3.636,35</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>Restam 9 unid.</t>
-        </is>
+      <c r="B47" t="n">
+        <v>2899.99</v>
+      </c>
+      <c r="C47" t="n">
+        <v>3636.35</v>
+      </c>
+      <c r="D47" t="n">
+        <v>9</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -2273,14 +2077,18 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Ultra 7-265KF,</t>
+          <t>Ultra 7</t>
         </is>
       </c>
       <c r="G47" t="n">
         <v>5.5</v>
       </c>
-      <c r="H47" t="inlineStr"/>
-      <c r="I47" t="inlineStr"/>
+      <c r="H47" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I47" t="n">
+        <v>27.5</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2288,20 +2096,14 @@
           <t>Processador Intel Core i9-13900, 5.6GHz Max Turbo, Cache 36MB, 24 Núcleos, 32 Threads, LGA 1700, Vídeo Integrado - BX8071513900</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>3.949,99</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>5.555,54</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Restam 10 unid.</t>
-        </is>
+      <c r="B48" t="n">
+        <v>3949.99</v>
+      </c>
+      <c r="C48" t="n">
+        <v>5555.54</v>
+      </c>
+      <c r="D48" t="n">
+        <v>10</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -2310,13 +2112,15 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Core i9-13900,</t>
+          <t>Core i9-13900</t>
         </is>
       </c>
       <c r="G48" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H48" t="n">
         <v>5.6</v>
       </c>
-      <c r="H48" t="inlineStr"/>
       <c r="I48" t="n">
         <v>36</v>
       </c>
@@ -2327,20 +2131,14 @@
           <t>Processador Intel Core Ultra 5-245KF, 5.2GHz, Até 14 Núcleos, Com suporte a PCIe 5.0 e 4.0 e suporte a DDR5 - BX80768245KF</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>1.999,99</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>2.840,90</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Restam 10 unid.</t>
-        </is>
+      <c r="B49" t="n">
+        <v>1999.99</v>
+      </c>
+      <c r="C49" t="n">
+        <v>2840.9</v>
+      </c>
+      <c r="D49" t="n">
+        <v>10</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -2349,14 +2147,18 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Ultra 5-245KF,</t>
+          <t>Ultra 5</t>
         </is>
       </c>
       <c r="G49" t="n">
         <v>5.2</v>
       </c>
-      <c r="H49" t="inlineStr"/>
-      <c r="I49" t="inlineStr"/>
+      <c r="H49" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I49" t="n">
+        <v>27.5</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2364,20 +2166,14 @@
           <t>Processador AMD Ryzen 9 9950x, 4.3GHz (5.7ghz Turbo) Cache 16MB, AM5, 16 Nucleos, 32 Threads, Radeon Graphics, Sem Cooler - 100-100001277wof</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>4.434,93</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>5.428,32</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Restam 22 unid.</t>
-        </is>
+      <c r="B50" t="n">
+        <v>4434.93</v>
+      </c>
+      <c r="C50" t="n">
+        <v>5428.32</v>
+      </c>
+      <c r="D50" t="n">
+        <v>22</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -2386,13 +2182,15 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Ryzen 9 9950x,</t>
+          <t>Ryzen 9 9950x</t>
         </is>
       </c>
       <c r="G50" t="n">
         <v>4.3</v>
       </c>
-      <c r="H50" t="inlineStr"/>
+      <c r="H50" t="n">
+        <v>5.05</v>
+      </c>
       <c r="I50" t="n">
         <v>16</v>
       </c>
@@ -2403,20 +2201,14 @@
           <t>Processador Intel Core I7 14700k, 5.60ghz Max Turbo, 20-core, 28-threads, LGA 1700</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>2.769,00</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>3.437,90</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>Restam 61 unid.</t>
-        </is>
+      <c r="B51" t="n">
+        <v>2769</v>
+      </c>
+      <c r="C51" t="n">
+        <v>3437.9</v>
+      </c>
+      <c r="D51" t="n">
+        <v>61</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2425,12 +2217,18 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Core I7 14700k,</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr"/>
-      <c r="H51" t="inlineStr"/>
-      <c r="I51" t="inlineStr"/>
+          <t>Core I7 14700k</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H51" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="I51" t="n">
+        <v>27.5</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2438,20 +2236,14 @@
           <t>Processador Intel Core i3-13100F, 4.5GHz Max Turbo, Cache 12MB, 4 Núcleos, 8 Threads, LGA 1700 - BX8071513100F</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>649,99</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>772,72</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Restam 2 unid.</t>
-        </is>
+      <c r="B52" t="n">
+        <v>649.99</v>
+      </c>
+      <c r="C52" t="n">
+        <v>772.72</v>
+      </c>
+      <c r="D52" t="n">
+        <v>2</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2460,13 +2252,15 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Core i3-13100F,</t>
+          <t>Core i3-13100F</t>
         </is>
       </c>
       <c r="G52" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H52" t="n">
         <v>4.5</v>
       </c>
-      <c r="H52" t="inlineStr"/>
       <c r="I52" t="n">
         <v>12</v>
       </c>
@@ -2477,20 +2271,14 @@
           <t>Processador Intel Core Ultra 7 265k Arrow Lake 3.9ghz 5.5ghz Turbo 20cores 20threads LGA 1851 Video Integrado</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>2.669,00</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>3.321,90</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Restam 17 unid.</t>
-        </is>
+      <c r="B53" t="n">
+        <v>2669</v>
+      </c>
+      <c r="C53" t="n">
+        <v>3321.9</v>
+      </c>
+      <c r="D53" t="n">
+        <v>17</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2502,9 +2290,15 @@
           <t>Ultra 7</t>
         </is>
       </c>
-      <c r="G53" t="inlineStr"/>
-      <c r="H53" t="inlineStr"/>
-      <c r="I53" t="inlineStr"/>
+      <c r="G53" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="H53" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I53" t="n">
+        <v>27.5</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2512,20 +2306,14 @@
           <t>Processador Intel Core I9-13900kf, Lga 1700, 36MB Cache - Bx8071513900kf</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>3.379,00</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>4.106,90</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>Restam 11 unid.</t>
-        </is>
+      <c r="B54" t="n">
+        <v>3379</v>
+      </c>
+      <c r="C54" t="n">
+        <v>4106.9</v>
+      </c>
+      <c r="D54" t="n">
+        <v>11</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2534,12 +2322,18 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Core I9-1</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr"/>
-      <c r="H54" t="inlineStr"/>
-      <c r="I54" t="inlineStr"/>
+          <t>Core I9-13900kf</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H54" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I54" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2547,20 +2341,14 @@
           <t>Processador Intel Core I9 14900k, 14ª Geração, 3.6 GHZ 6.0 GHZ Turbo, Cache 36MB, Intel LGA1700 - BX8071514900K</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>3.649,00</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>4.403,90</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>Restam 59 unid.</t>
-        </is>
+      <c r="B55" t="n">
+        <v>3649</v>
+      </c>
+      <c r="C55" t="n">
+        <v>4403.9</v>
+      </c>
+      <c r="D55" t="n">
+        <v>59</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -2569,11 +2357,15 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Core I9 14900k,</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr"/>
-      <c r="H55" t="inlineStr"/>
+          <t>Core I9 14900k</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="H55" t="n">
+        <v>5.05</v>
+      </c>
       <c r="I55" t="n">
         <v>36</v>
       </c>
@@ -2584,20 +2376,14 @@
           <t>Processador Intel Core I5 13400 Box Lga 1700 10 Cores 16 Threads 20MB Cache - BX8071513400</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>1.289,00</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>1.544,90</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>Restam 77 unid.</t>
-        </is>
+      <c r="B56" t="n">
+        <v>1289</v>
+      </c>
+      <c r="C56" t="n">
+        <v>1544.9</v>
+      </c>
+      <c r="D56" t="n">
+        <v>77</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2609,9 +2395,15 @@
           <t>Core I5 13400</t>
         </is>
       </c>
-      <c r="G56" t="inlineStr"/>
-      <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr"/>
+      <c r="G56" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H56" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I56" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2619,20 +2411,14 @@
           <t>Processador Intel Core I7-13700f, 2,10 GHz (5.2GHz Max Turbo) Cache 30MB, 16 Núcleos, 24 Threads, Sem Vídeo Integrado - Bx8071513700f</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>2.299,00</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>2.755,90</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>Restam 18 unid.</t>
-        </is>
+      <c r="B57" t="n">
+        <v>2299</v>
+      </c>
+      <c r="C57" t="n">
+        <v>2755.9</v>
+      </c>
+      <c r="D57" t="n">
+        <v>18</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2641,11 +2427,11 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Core I7-1</t>
+          <t>Core I7-13700f</t>
         </is>
       </c>
       <c r="G57" t="n">
-        <v>10</v>
+        <v>2.1</v>
       </c>
       <c r="H57" t="n">
         <v>5.2</v>
@@ -2660,20 +2446,14 @@
           <t>Processador Intel Core I9 14900f, 5.80ghz, Max Turbo, 24-core, 32-threads, LGA1700</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>4.209,00</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>5.098,90</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>Restam 17 unid.</t>
-        </is>
+      <c r="B58" t="n">
+        <v>4209</v>
+      </c>
+      <c r="C58" t="n">
+        <v>5098.9</v>
+      </c>
+      <c r="D58" t="n">
+        <v>17</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -2682,12 +2462,18 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Core I9 14900f,</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr"/>
-      <c r="H58" t="inlineStr"/>
-      <c r="I58" t="inlineStr"/>
+          <t>Core I9 14900f</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H58" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I58" t="n">
+        <v>27.5</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2695,20 +2481,14 @@
           <t>Processador Intel Core I7-12700K, 3.6GHz (5.0GHz Max Turbo), Cache 25MB, LGA 1700 - BX8071512700K</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>1.929,00</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>2.330,90</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>Restam 89 unid.</t>
-        </is>
+      <c r="B59" t="n">
+        <v>1929</v>
+      </c>
+      <c r="C59" t="n">
+        <v>2330.9</v>
+      </c>
+      <c r="D59" t="n">
+        <v>89</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -2717,7 +2497,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Core I7-1</t>
+          <t>Core I7-12700K</t>
         </is>
       </c>
       <c r="G59" t="n">
@@ -2736,20 +2516,14 @@
           <t>Processador Intel Core I9 14900, 5.80ghz, Max Turbo, 24-core, 32-threads, LGA1700</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>3.969,00</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>5.072,90</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>Restam 30 unid.</t>
-        </is>
+      <c r="B60" t="n">
+        <v>3969</v>
+      </c>
+      <c r="C60" t="n">
+        <v>5072.9</v>
+      </c>
+      <c r="D60" t="n">
+        <v>30</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -2758,12 +2532,18 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Core I9 14900,</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr"/>
-      <c r="H60" t="inlineStr"/>
-      <c r="I60" t="inlineStr"/>
+          <t>Core I9 14900</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H60" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I60" t="n">
+        <v>27.5</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2771,20 +2551,14 @@
           <t>Processador Intel Core I9 14900kf, 14ª Geração, 3.6 Ghz (6.0ghz Turbo), Cache 36MB, LGA 1700 - BX8071514900KF</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>3.359,00</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>4.079,90</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>Restam 70 unid.</t>
-        </is>
+      <c r="B61" t="n">
+        <v>3359</v>
+      </c>
+      <c r="C61" t="n">
+        <v>4079.9</v>
+      </c>
+      <c r="D61" t="n">
+        <v>70</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2793,11 +2567,15 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Core I9 14900kf,</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr"/>
-      <c r="H61" t="inlineStr"/>
+          <t>Core I9 14900kf</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="H61" t="n">
+        <v>5.05</v>
+      </c>
       <c r="I61" t="n">
         <v>36</v>
       </c>
@@ -2808,20 +2586,14 @@
           <t>Processador Intel Core I9 13900K, 5.80GHz Max Turbo, Cache 36MB, Quad Core, 32 Threads, LGA 1700</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>4.779,00</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>5.909,90</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>Restam 2 unid.</t>
-        </is>
+      <c r="B62" t="n">
+        <v>4779</v>
+      </c>
+      <c r="C62" t="n">
+        <v>5909.9</v>
+      </c>
+      <c r="D62" t="n">
+        <v>2</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -2830,13 +2602,15 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Core I9 13900K,</t>
+          <t>Core I9 13900K</t>
         </is>
       </c>
       <c r="G62" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H62" t="n">
         <v>5.8</v>
       </c>
-      <c r="H62" t="inlineStr"/>
       <c r="I62" t="n">
         <v>36</v>
       </c>
@@ -2847,20 +2621,14 @@
           <t>Processador Intel Core I9 13900f, 2.00ghz, 24-core, LGA1700</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>2.999,00</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>3.617,90</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>Restam 13 unid.</t>
-        </is>
+      <c r="B63" t="n">
+        <v>2999</v>
+      </c>
+      <c r="C63" t="n">
+        <v>3617.9</v>
+      </c>
+      <c r="D63" t="n">
+        <v>13</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2869,12 +2637,18 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Core I9 13900f,</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr"/>
-      <c r="H63" t="inlineStr"/>
-      <c r="I63" t="inlineStr"/>
+          <t>Core I9 13900f</t>
+        </is>
+      </c>
+      <c r="G63" t="n">
+        <v>2</v>
+      </c>
+      <c r="H63" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I63" t="n">
+        <v>27.5</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2882,20 +2656,14 @@
           <t>Processador AMD Ryzen Threadripper Pro 5975WX, Cache 128MB, 32 Núcleos, SP3 WOF - 100-100000445WOF</t>
         </is>
       </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>17.499,99</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>27.433,64</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>Restam 2 unid.</t>
-        </is>
+      <c r="B64" t="n">
+        <v>17499.99</v>
+      </c>
+      <c r="C64" t="n">
+        <v>27433.64</v>
+      </c>
+      <c r="D64" t="n">
+        <v>2</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2904,11 +2672,15 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Desconhecido</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr"/>
-      <c r="H64" t="inlineStr"/>
+          <t>Threadripper Pro 5975WX</t>
+        </is>
+      </c>
+      <c r="G64" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H64" t="n">
+        <v>5.05</v>
+      </c>
       <c r="I64" t="n">
         <v>128</v>
       </c>
@@ -2919,20 +2691,14 @@
           <t>Processador AMD Ryzen Threadripper Pro 5965WX, Cache 128 MB, 24 Núcleos, SP3 - 100-100000446WOF</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>10.999,99</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>19.982,53</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>Restam 1 unid.</t>
-        </is>
+      <c r="B65" t="n">
+        <v>10999.99</v>
+      </c>
+      <c r="C65" t="n">
+        <v>19982.53</v>
+      </c>
+      <c r="D65" t="n">
+        <v>1</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2941,12 +2707,18 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Desconhecido</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr"/>
-      <c r="H65" t="inlineStr"/>
-      <c r="I65" t="inlineStr"/>
+          <t>Threadripper Pro 5965WX</t>
+        </is>
+      </c>
+      <c r="G65" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H65" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I65" t="n">
+        <v>128</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2954,20 +2726,14 @@
           <t>Processador Intel Ultra 5 245kf Arrow Lake 4.2ghz 5.2ghz Turbo 14cores 214threads LGA 1851 S/video S/cooler</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>2.349,00</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>2.896,90</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>Restam 18 unid.</t>
-        </is>
+      <c r="B66" t="n">
+        <v>2349</v>
+      </c>
+      <c r="C66" t="n">
+        <v>2896.9</v>
+      </c>
+      <c r="D66" t="n">
+        <v>18</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2979,9 +2745,15 @@
           <t>Ultra 5</t>
         </is>
       </c>
-      <c r="G66" t="inlineStr"/>
-      <c r="H66" t="inlineStr"/>
-      <c r="I66" t="inlineStr"/>
+      <c r="G66" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="H66" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I66" t="n">
+        <v>27.5</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2989,20 +2761,14 @@
           <t>Processador AMD Ryzen Threadripper Pro 5995WX, Cache 256 MB, 64 Núcleos, SP3 WOF - 100-100000444WOF</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>37.999,99</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>52.941,16</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>Restam 1 unid.</t>
-        </is>
+      <c r="B67" t="n">
+        <v>37999.99</v>
+      </c>
+      <c r="C67" t="n">
+        <v>52941.16</v>
+      </c>
+      <c r="D67" t="n">
+        <v>1</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -3011,12 +2777,18 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Desconhecido</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr"/>
-      <c r="H67" t="inlineStr"/>
-      <c r="I67" t="inlineStr"/>
+          <t>Threadripper Pro 5995WX</t>
+        </is>
+      </c>
+      <c r="G67" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H67" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I67" t="n">
+        <v>256</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3024,20 +2796,14 @@
           <t>Processador Intel Core I9-12900KF, 3.2GHz, Cache 30MB, Hexa Core, 24 Threads, LGA 1700 - BX8071512900KF</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>2.979,00</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>3.591,90</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>Restam 2 unid.</t>
-        </is>
+      <c r="B68" t="n">
+        <v>2979</v>
+      </c>
+      <c r="C68" t="n">
+        <v>3591.9</v>
+      </c>
+      <c r="D68" t="n">
+        <v>2</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3046,13 +2812,15 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Core I9-1</t>
+          <t>Core I9-12900KF</t>
         </is>
       </c>
       <c r="G68" t="n">
         <v>3.2</v>
       </c>
-      <c r="H68" t="inlineStr"/>
+      <c r="H68" t="n">
+        <v>5.05</v>
+      </c>
       <c r="I68" t="n">
         <v>30</v>
       </c>
@@ -3063,20 +2831,14 @@
           <t>Processador Intel Pentium Gold G6405, 10ª Geração, 4.10GHz, Dual Core, 4 Threads, LGA 1200 - BX80701G6405</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>509,00</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>617,90</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>Restam 95 unid.</t>
-        </is>
+      <c r="B69" t="n">
+        <v>509</v>
+      </c>
+      <c r="C69" t="n">
+        <v>617.9</v>
+      </c>
+      <c r="D69" t="n">
+        <v>95</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3091,8 +2853,12 @@
       <c r="G69" t="n">
         <v>4.1</v>
       </c>
-      <c r="H69" t="inlineStr"/>
-      <c r="I69" t="inlineStr"/>
+      <c r="H69" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I69" t="n">
+        <v>27.5</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3100,20 +2866,14 @@
           <t>Processador Intel Core Ultra 7 265kf Arrow Lake 3.9ghz 5.5ghz</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>2.669,00</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>3.270,90</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>Restam 23 unid.</t>
-        </is>
+      <c r="B70" t="n">
+        <v>2669</v>
+      </c>
+      <c r="C70" t="n">
+        <v>3270.9</v>
+      </c>
+      <c r="D70" t="n">
+        <v>23</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -3125,9 +2885,15 @@
           <t>Ultra 7</t>
         </is>
       </c>
-      <c r="G70" t="inlineStr"/>
-      <c r="H70" t="inlineStr"/>
-      <c r="I70" t="inlineStr"/>
+      <c r="G70" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="H70" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I70" t="n">
+        <v>27.5</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3135,20 +2901,14 @@
           <t>Processador Intel Ultra 5 245k Arrow Lake 4.2ghz 5.2ghz Turbo 14cores 14threads LGA 1851 Video Integrado</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>2.469,00</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>3.051,90</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>Restam 20 unid.</t>
-        </is>
+      <c r="B71" t="n">
+        <v>2469</v>
+      </c>
+      <c r="C71" t="n">
+        <v>3051.9</v>
+      </c>
+      <c r="D71" t="n">
+        <v>20</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -3160,9 +2920,15 @@
           <t>Ultra 5</t>
         </is>
       </c>
-      <c r="G71" t="inlineStr"/>
-      <c r="H71" t="inlineStr"/>
-      <c r="I71" t="inlineStr"/>
+      <c r="G71" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="H71" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I71" t="n">
+        <v>27.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>